<commit_message>
Email functionality added to workflow
</commit_message>
<xml_diff>
--- a/Participants.xlsx
+++ b/Participants.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\6th sem\RPA\Course Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1365E2AA-F73A-4738-8BAF-28634B88D314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09FDE25-ADCD-4E78-BA62-0C31956BF4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6F9B4728-B97B-4819-A1C8-F25D729FF529}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -45,22 +44,19 @@
     <t>Aniket Saha</t>
   </si>
   <si>
-    <t>2gi19cs189@students.git.edu</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>X3</t>
+    <t>Madhumita Saha</t>
   </si>
   <si>
     <t>anikets349@gmail.com</t>
   </si>
   <si>
-    <t>aniket.saha279@gmail.com</t>
+    <t>madhumitasaha898@gmail.com</t>
+  </si>
+  <si>
+    <t>Abhijit Saha</t>
+  </si>
+  <si>
+    <t>abhijitsaha8698@gmail.com</t>
   </si>
   <si>
     <t>Akshay Deshpande</t>
@@ -456,16 +452,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEBC1EB-98EA-49CE-BEC0-5C20CA0B4C98}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -478,101 +474,65 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
+    <sortCondition ref="A1:A7"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B5B27A18-55B0-458A-89C6-BE01F450BBD0}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{87729EB4-D85F-42B2-BA38-ADDC473DFA12}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{C539585C-AE31-468E-9133-C2D6FA97E279}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{E4952E99-E3A9-4DCA-B7F9-639D6C6A2744}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{B5B27A18-55B0-458A-89C6-BE01F450BBD0}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{21CF6913-6E2F-467A-B4C4-2B93B1969D4C}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{EC828183-DFDB-4DC5-B944-F25AA804954C}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{512E22B9-ED0A-4E9A-9E60-B9987CB1A91F}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{3F94DBC1-ED99-4BA9-97BC-B652CF6B1449}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{D5CAF3CE-F33C-45D3-9130-5E603352CAF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3D0E9B-D254-4BAD-8138-68678F74767B}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{C11335D1-DDE0-4EFC-BFC8-06BBDF83F7D1}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{91CBB92B-C1C9-4E6D-A3CF-A87A81D6DBB4}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{33D037F3-F694-44CE-A81E-1CEF6CB21E82}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>